<commit_message>
Adicionei loginNavbar.css shop-homepage.css home.php dir:img jquery.js signUp.php
</commit_message>
<xml_diff>
--- a/tabelasProjeto.xlsx
+++ b/tabelasProjeto.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Possíveis Tabelas:</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userlevel </t>
   </si>
   <si>
     <t xml:space="preserve">address </t>
@@ -64,6 +67,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,6 +89,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -232,22 +237,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:H6"/>
+  <dimension ref="A3:I6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.66836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.2755102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.43367346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.30612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.64285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -266,6 +271,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -292,10 +298,13 @@
       <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A5:I5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>